<commit_message>
Site updated: 2023-01-18 19:28:52
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2023.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2023.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27400" windowHeight="14700" activeTab="1"/>
+    <workbookView windowHeight="15200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>角色</t>
   </si>
@@ -162,6 +162,21 @@
 3、欲望远离娱乐至死（消除所有娱乐至死的因素）</t>
   </si>
   <si>
+    <t>面试相关</t>
+  </si>
+  <si>
+    <t>一月计划：技术点阅读6遍、刷100道题、研究透彻设计模式（50%）、jvm考点系统性梳理、多线程实战场景梳理</t>
+  </si>
+  <si>
+    <t>进行中</t>
+  </si>
+  <si>
+    <t>二月计划：技术点阅读12遍、刷100道题、研究透彻业务设计模式DDD、研究透彻设计模式（50%）</t>
+  </si>
+  <si>
+    <t>三月计划：技术点阅读12遍、刷100道题、springboot、springcloud系统学习</t>
+  </si>
+  <si>
     <t>开始时间:</t>
   </si>
   <si>
@@ -183,7 +198,7 @@
     <t>技术广度的发力点</t>
   </si>
   <si>
-    <t>进行中</t>
+    <t>完成</t>
   </si>
   <si>
     <t>技术面深度发力点</t>
@@ -195,13 +210,34 @@
     <t>了解公考</t>
   </si>
   <si>
+    <t>知识点温习一遍</t>
+  </si>
+  <si>
+    <t>刷题20</t>
+  </si>
+  <si>
+    <t>JVM考点系统性梳理</t>
+  </si>
+  <si>
     <t>第二周</t>
   </si>
   <si>
+    <t>知识点温习2遍</t>
+  </si>
+  <si>
+    <t>多线程实战-完成50%</t>
+  </si>
+  <si>
     <t>第三周</t>
   </si>
   <si>
     <t>第四周</t>
+  </si>
+  <si>
+    <t>刷题40</t>
+  </si>
+  <si>
+    <t>研究透彻设计模式（50%）</t>
   </si>
 </sst>
 </file>
@@ -209,9 +245,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -223,14 +259,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,6 +281,60 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -251,22 +342,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,7 +379,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -289,23 +387,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,60 +408,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="41">
     <fill>
@@ -400,6 +436,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -412,12 +454,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -436,186 +472,186 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -887,6 +923,19 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
         <color indexed="14"/>
       </right>
       <top style="thin">
@@ -916,6 +965,56 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -926,7 +1025,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -960,207 +1059,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="31" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1197,6 +1246,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1221,16 +1276,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1239,7 +1297,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1275,10 +1333,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2506,200 +2573,200 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:5">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:5">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:5">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
     </row>
     <row r="5" ht="14" customHeight="1" spans="1:5">
-      <c r="A5" s="42"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" ht="14" customHeight="1" spans="1:5">
-      <c r="A6" s="42"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:5">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
     </row>
     <row r="8" ht="14" customHeight="1" spans="1:5">
-      <c r="A8" s="42"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:5">
-      <c r="A9" s="42"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" ht="14" customHeight="1" spans="1:5">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
     </row>
     <row r="11" ht="14" customHeight="1" spans="1:5">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:5">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
     </row>
     <row r="13" ht="14" customHeight="1" spans="1:5">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:5">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:5">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:5">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
     </row>
     <row r="17" ht="14" customHeight="1" spans="1:5">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
     </row>
     <row r="18" ht="14" customHeight="1" spans="1:5">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
     </row>
     <row r="19" ht="14" customHeight="1" spans="1:5">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
     </row>
     <row r="20" ht="14" customHeight="1" spans="1:5">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
     </row>
     <row r="21" ht="14" customHeight="1" spans="1:5">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
     </row>
     <row r="22" ht="14" customHeight="1" spans="1:5">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
     </row>
     <row r="23" ht="14" customHeight="1" spans="1:5">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2719,176 +2786,208 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="16.3557692307692" style="1" customWidth="1"/>
-    <col min="2" max="2" width="99.1153846153846" style="20" customWidth="1"/>
+    <col min="2" max="2" width="99.1153846153846" style="23" customWidth="1"/>
     <col min="3" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="26" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="27" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:3">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="36" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:3">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="36" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:3">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="36" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:3">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="40" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" ht="73" customHeight="1" spans="1:3">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="42" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="15" customHeight="1" spans="1:3">
+      <c r="A15" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:3">
+      <c r="A16" s="43"/>
+      <c r="B16" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:3">
+      <c r="A17" s="43"/>
+      <c r="B17" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:A17"/>
+  </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C7 C8 C14 C2:C5 C9:C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C7 C8 C14 C15 C16 C17 C2:C5 C9:C13">
       <formula1>"未进行,进行中,已暂停,已完成"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2905,12 +3004,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
@@ -2920,7 +3019,7 @@
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3">
         <v>20220401</v>
@@ -2929,12 +3028,12 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B2" s="6">
         <v>20220430</v>
@@ -2943,12 +3042,12 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
       <c r="A3" s="8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>1</v>
@@ -2966,105 +3065,119 @@
         <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
       <c r="A4" s="10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="19" t="s">
-        <v>54</v>
+      <c r="G4" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="H4" s="11"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
       <c r="A5" s="12"/>
       <c r="B5" s="11" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="19" t="s">
-        <v>54</v>
+      <c r="G5" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="H5" s="11"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
       <c r="A6" s="12"/>
       <c r="B6" s="11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="19" t="s">
-        <v>54</v>
+      <c r="G6" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
       <c r="A7" s="12"/>
       <c r="B7" s="11" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="19" t="s">
-        <v>54</v>
+      <c r="G7" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="H7" s="11"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" spans="1:8">
       <c r="A8" s="13"/>
-      <c r="B8" s="11"/>
+      <c r="B8" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="G8" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="H8" s="11"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A9" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="11"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="G9" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" ht="13.35" customHeight="1" spans="1:8">
+    <row r="10" ht="13.65" customHeight="1" spans="1:8">
       <c r="A10" s="12"/>
-      <c r="B10" s="11"/>
+      <c r="B10" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="G10" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="H10" s="11"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A11" s="13"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
@@ -3072,11 +3185,11 @@
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="11"/>
+    <row r="12" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A12" s="14"/>
+      <c r="B12" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
@@ -3085,8 +3198,10 @@
       <c r="H12" s="11"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A13" s="12"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -3094,9 +3209,13 @@
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" ht="14" customHeight="1" spans="1:8">
-      <c r="A14" s="13"/>
-      <c r="B14" s="11"/>
+    <row r="14" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A14" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -3105,10 +3224,10 @@
       <c r="H14" s="11"/>
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A15" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="11"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
@@ -3116,9 +3235,11 @@
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A16" s="12"/>
-      <c r="B16" s="11"/>
+    <row r="16" ht="14" customHeight="1" spans="1:8">
+      <c r="A16" s="15"/>
+      <c r="B16" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
@@ -3127,8 +3248,12 @@
       <c r="H16" s="11"/>
     </row>
     <row r="17" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A17" s="13"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
@@ -3136,9 +3261,11 @@
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" ht="13.65" customHeight="1" spans="1:8">
+    <row r="18" ht="13.35" customHeight="1" spans="1:8">
       <c r="A18" s="14"/>
-      <c r="B18" s="11"/>
+      <c r="B18" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
@@ -3146,12 +3273,34 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
     </row>
+    <row r="19" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A19" s="15"/>
+      <c r="B19" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A20" s="16"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A17:A19"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>

</xml_diff>

<commit_message>
Site updated: 2023-06-15 19:29:22
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2023.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2023.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15200" activeTab="2"/>
+    <workbookView windowHeight="17040" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
     <sheet name="待办任务" sheetId="3" r:id="rId2"/>
     <sheet name="一月" sheetId="10" r:id="rId3"/>
+    <sheet name="二月" sheetId="11" r:id="rId4"/>
+    <sheet name="五月" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="83">
   <si>
     <t>角色</t>
   </si>
@@ -124,6 +126,9 @@
   </si>
   <si>
     <t>拥有居住证后，儿童可以在上海享受哪些福利？儿童医保/儿童互助基金…</t>
+  </si>
+  <si>
+    <t>思考是否要考公务员</t>
   </si>
   <si>
     <t>掌握考公的套路</t>
@@ -165,16 +170,22 @@
     <t>面试相关</t>
   </si>
   <si>
-    <t>一月计划：技术点阅读6遍、刷100道题、研究透彻设计模式（50%）、jvm考点系统性梳理、多线程实战场景梳理</t>
+    <t>研究透彻设计模式（50%）、jvm考点系统性梳理、多线程实战场景梳理</t>
   </si>
   <si>
     <t>进行中</t>
   </si>
   <si>
-    <t>二月计划：技术点阅读12遍、刷100道题、研究透彻业务设计模式DDD、研究透彻设计模式（50%）</t>
-  </si>
-  <si>
-    <t>三月计划：技术点阅读12遍、刷100道题、springboot、springcloud系统学习</t>
+    <t>研究透彻业务设计模式DDD、研究透彻设计模式（50%）</t>
+  </si>
+  <si>
+    <t>springboot、springcloud系统学习</t>
+  </si>
+  <si>
+    <t>学习备忘中的学习内容完成</t>
+  </si>
+  <si>
+    <t>学习知识点“精”、“简”</t>
   </si>
   <si>
     <t>开始时间:</t>
@@ -210,6 +221,9 @@
     <t>了解公考</t>
   </si>
   <si>
+    <t>未完成</t>
+  </si>
+  <si>
     <t>知识点温习一遍</t>
   </si>
   <si>
@@ -238,6 +252,24 @@
   </si>
   <si>
     <t>研究透彻设计模式（50%）</t>
+  </si>
+  <si>
+    <t>刷题100</t>
+  </si>
+  <si>
+    <t>知识点温习一遍-3.5小时/每周</t>
+  </si>
+  <si>
+    <t>刷题70</t>
+  </si>
+  <si>
+    <t>看书3.5小时/每周</t>
+  </si>
+  <si>
+    <t>整理5篇知识点精简</t>
+  </si>
+  <si>
+    <t>看5篇知识点</t>
   </si>
 </sst>
 </file>
@@ -247,10 +279,10 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -258,16 +290,37 @@
       <charset val="134"/>
     </font>
     <font>
+      <strike/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,8 +333,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,9 +397,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -311,9 +411,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,22 +433,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -357,53 +457,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -436,13 +490,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.6"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.6"/>
+        <fgColor theme="6" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,6 +526,120 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -484,13 +652,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,19 +682,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,127 +694,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -797,6 +851,21 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="17"/>
       </left>
       <right style="thin">
@@ -837,21 +906,6 @@
       </top>
       <bottom style="thin">
         <color indexed="17"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="18"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -965,7 +1019,66 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -986,17 +1099,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1011,205 +1113,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="31" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1249,62 +1303,71 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1333,14 +1396,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2573,200 +2639,200 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:5">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:5">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:5">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
     </row>
     <row r="5" ht="14" customHeight="1" spans="1:5">
-      <c r="A5" s="48"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
     </row>
     <row r="6" ht="14" customHeight="1" spans="1:5">
-      <c r="A6" s="48"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:5">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
     </row>
     <row r="8" ht="14" customHeight="1" spans="1:5">
-      <c r="A8" s="48"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:5">
-      <c r="A9" s="48"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
     </row>
     <row r="10" ht="14" customHeight="1" spans="1:5">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
     </row>
     <row r="11" ht="14" customHeight="1" spans="1:5">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:5">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
     </row>
     <row r="13" ht="14" customHeight="1" spans="1:5">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:5">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:5">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:5">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
     </row>
     <row r="17" ht="14" customHeight="1" spans="1:5">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
     </row>
     <row r="18" ht="14" customHeight="1" spans="1:5">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
     </row>
     <row r="19" ht="14" customHeight="1" spans="1:5">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
     </row>
     <row r="20" ht="14" customHeight="1" spans="1:5">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
     </row>
     <row r="21" ht="14" customHeight="1" spans="1:5">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
     </row>
     <row r="22" ht="14" customHeight="1" spans="1:5">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
     </row>
     <row r="23" ht="14" customHeight="1" spans="1:5">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2786,208 +2852,235 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="16.3557692307692" style="1" customWidth="1"/>
-    <col min="2" max="2" width="99.1153846153846" style="23" customWidth="1"/>
+    <col min="2" max="2" width="99.1153846153846" style="24" customWidth="1"/>
     <col min="3" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="30" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" ht="13.35" customHeight="1" spans="1:3">
+      <c r="A10" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" customHeight="1" spans="1:3">
-      <c r="A10" s="34" t="s">
+      <c r="B10" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:3">
       <c r="A11" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="C11" s="39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:3">
+      <c r="A12" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="B12" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" customHeight="1" spans="1:3">
-      <c r="A12" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="36" t="s">
+    <row r="13" customHeight="1" spans="1:3">
+      <c r="A13" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" customHeight="1" spans="1:3">
-      <c r="A13" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="39" t="s">
+    <row r="14" customHeight="1" spans="1:3">
+      <c r="A14" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="B14" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" ht="73" customHeight="1" spans="1:3">
-      <c r="A14" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="39" t="s">
+    <row r="15" ht="73" customHeight="1" spans="1:3">
+      <c r="A15" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="B15" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" customHeight="1" spans="1:3">
-      <c r="A15" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="35" t="s">
+    <row r="16" customHeight="1" spans="1:3">
+      <c r="A16" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="B16" s="38" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" customHeight="1" spans="1:3">
-      <c r="A16" s="43"/>
-      <c r="B16" s="35" t="s">
+      <c r="C16" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="36" t="s">
+    </row>
+    <row r="17" customHeight="1" spans="1:3">
+      <c r="A17" s="46"/>
+      <c r="B17" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="47" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" customHeight="1" spans="1:3">
-      <c r="A17" s="43"/>
-      <c r="B17" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="36" t="s">
+    <row r="18" customHeight="1" spans="1:3">
+      <c r="A18" s="46"/>
+      <c r="B18" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="1:3">
+      <c r="A19" s="46"/>
+      <c r="B19" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:3">
+      <c r="A20" s="46"/>
+      <c r="B20" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="47" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A16:A20"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C7 C8 C14 C15 C16 C17 C2:C5 C9:C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C7 C8 C9 C15 C16 C17 C18 C19 C20 C2:C5 C10:C14">
       <formula1>"未进行,进行中,已暂停,已完成"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3006,10 +3099,10 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <selection pane="topRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
@@ -3019,7 +3112,7 @@
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3">
         <v>20220401</v>
@@ -3028,12 +3121,12 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B2" s="6">
         <v>20220430</v>
@@ -3042,12 +3135,12 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
       <c r="A3" s="8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>1</v>
@@ -3065,228 +3158,246 @@
         <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
       <c r="A4" s="10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="21" t="s">
-        <v>59</v>
+      <c r="G4" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="H4" s="11"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
       <c r="A5" s="12"/>
       <c r="B5" s="11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="21" t="s">
-        <v>59</v>
+      <c r="G5" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="H5" s="11"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
       <c r="A6" s="12"/>
       <c r="B6" s="11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="21" t="s">
-        <v>59</v>
+      <c r="G6" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
       <c r="A7" s="12"/>
       <c r="B7" s="11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="22" t="s">
-        <v>49</v>
+      <c r="G7" s="20" t="s">
+        <v>66</v>
       </c>
       <c r="H7" s="11"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A8" s="13"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="21" t="s">
-        <v>59</v>
+      <c r="G8" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="H8" s="11"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
       <c r="A9" s="12"/>
       <c r="B9" s="11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="21" t="s">
-        <v>59</v>
+      <c r="G9" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="H9" s="11"/>
     </row>
     <row r="10" ht="13.65" customHeight="1" spans="1:8">
       <c r="A10" s="12"/>
       <c r="B10" s="11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="21" t="s">
-        <v>59</v>
+      <c r="G10" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="H10" s="11"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
       <c r="A11" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="G11" s="22" t="s">
+        <v>62</v>
+      </c>
       <c r="H11" s="11"/>
     </row>
     <row r="12" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="G12" s="22" t="s">
+        <v>62</v>
+      </c>
       <c r="H12" s="11"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A13" s="15"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="G13" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="H13" s="11"/>
     </row>
     <row r="14" ht="13.65" customHeight="1" spans="1:8">
       <c r="A14" s="10" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="G14" s="22" t="s">
+        <v>62</v>
+      </c>
       <c r="H14" s="11"/>
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A15" s="14"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
+      <c r="G15" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="H15" s="11"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:8">
-      <c r="A16" s="15"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="G16" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="H16" s="11"/>
     </row>
     <row r="17" ht="13.65" customHeight="1" spans="1:8">
       <c r="A17" s="10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="G17" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="H17" s="11"/>
     </row>
     <row r="18" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A18" s="14"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="G18" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="H18" s="11"/>
     </row>
     <row r="19" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A19" s="15"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="G19" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="H19" s="11"/>
     </row>
     <row r="20" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A20" s="16"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -3308,4 +3419,513 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14" customHeight="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3">
+        <v>20220401</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" ht="14" customHeight="1" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6">
+        <v>20220430</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" ht="14" customHeight="1" spans="1:8">
+      <c r="A3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A5" s="12"/>
+      <c r="B5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A6" s="12"/>
+      <c r="B6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A8" s="13"/>
+      <c r="B8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A9" s="14"/>
+      <c r="B9" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A11" s="13"/>
+      <c r="B11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" ht="14" customHeight="1" spans="1:8">
+      <c r="A12" s="14"/>
+      <c r="B12" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A15" s="14"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A16" s="15"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A15"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14" customHeight="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3">
+        <v>20220501</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" ht="14" customHeight="1" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6">
+        <v>20220531</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" ht="14" customHeight="1" spans="1:8">
+      <c r="A3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A6" s="12"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A8" s="13"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A9" s="14"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A11" s="13"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" ht="14" customHeight="1" spans="1:8">
+      <c r="A12" s="14"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A15" s="14"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A16" s="15"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A15"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6">
+      <formula1>"未进行,进行中,已暂停,已完成"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Site updated: 2023-07-12 21:38:46
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2023.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2023.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17040" activeTab="4"/>
+    <workbookView windowHeight="17020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="87">
   <si>
     <t>角色</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>学习知识点“精”、“简”</t>
+  </si>
+  <si>
+    <t>mac电脑学习备忘整理</t>
+  </si>
+  <si>
+    <t>如何拥有健康的身体</t>
+  </si>
+  <si>
+    <t>如何了解自己</t>
+  </si>
+  <si>
+    <t>如何利用ai改变行业</t>
   </si>
   <si>
     <t>开始时间:</t>
@@ -277,9 +289,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -333,14 +345,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
@@ -357,17 +361,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -379,19 +376,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -403,31 +392,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,9 +417,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -462,6 +429,51 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="41">
     <fill>
@@ -532,13 +544,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,19 +622,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,31 +670,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,49 +682,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,43 +712,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1034,30 +1046,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1073,13 +1061,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1113,144 +1105,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2852,14 +2864,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
@@ -3073,6 +3085,26 @@
       </c>
       <c r="C20" s="47" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="2:2">
+      <c r="B21" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="2:2">
+      <c r="B22" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" customHeight="1" spans="2:2">
+      <c r="B23" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" customHeight="1" spans="2:2">
+      <c r="B24" s="24" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3112,7 +3144,7 @@
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3">
         <v>20220401</v>
@@ -3126,7 +3158,7 @@
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B2" s="6">
         <v>20220430</v>
@@ -3140,7 +3172,7 @@
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>1</v>
@@ -3158,241 +3190,241 @@
         <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
       <c r="A4" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H4" s="11"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
       <c r="A5" s="12"/>
       <c r="B5" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H5" s="11"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
       <c r="A6" s="12"/>
       <c r="B6" s="11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
       <c r="A7" s="12"/>
       <c r="B7" s="11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H7" s="11"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" spans="1:8">
       <c r="A8" s="23"/>
       <c r="B8" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H8" s="11"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
       <c r="A9" s="12"/>
       <c r="B9" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H9" s="11"/>
     </row>
     <row r="10" ht="13.65" customHeight="1" spans="1:8">
       <c r="A10" s="12"/>
       <c r="B10" s="11" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H10" s="11"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
       <c r="A11" s="10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H11" s="11"/>
     </row>
     <row r="12" ht="13.35" customHeight="1" spans="1:8">
       <c r="A12" s="13"/>
       <c r="B12" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H12" s="11"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
       <c r="A13" s="14"/>
       <c r="B13" s="11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H13" s="11"/>
     </row>
     <row r="14" ht="13.65" customHeight="1" spans="1:8">
       <c r="A14" s="10" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H14" s="11"/>
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
       <c r="A15" s="13"/>
       <c r="B15" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H15" s="11"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:8">
       <c r="A16" s="14"/>
       <c r="B16" s="11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H16" s="11"/>
     </row>
     <row r="17" ht="13.65" customHeight="1" spans="1:8">
       <c r="A17" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H17" s="11"/>
     </row>
     <row r="18" ht="13.35" customHeight="1" spans="1:8">
       <c r="A18" s="13"/>
       <c r="B18" s="11" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H18" s="11"/>
     </row>
     <row r="19" ht="13.65" customHeight="1" spans="1:8">
       <c r="A19" s="14"/>
       <c r="B19" s="11" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H19" s="11"/>
     </row>
@@ -3441,7 +3473,7 @@
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3">
         <v>20220401</v>
@@ -3455,7 +3487,7 @@
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B2" s="6">
         <v>20220430</v>
@@ -3469,7 +3501,7 @@
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>1</v>
@@ -3487,147 +3519,147 @@
         <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
       <c r="A4" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H4" s="11"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
       <c r="A5" s="12"/>
       <c r="B5" s="11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H5" s="11"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
       <c r="A6" s="12"/>
       <c r="B6" s="11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" ht="13.65" customHeight="1" spans="1:8">
       <c r="A7" s="10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H7" s="11"/>
     </row>
     <row r="8" ht="13.35" customHeight="1" spans="1:8">
       <c r="A8" s="13"/>
       <c r="B8" s="11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H8" s="11"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
       <c r="A9" s="14"/>
       <c r="B9" s="11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H9" s="11"/>
     </row>
     <row r="10" ht="13.65" customHeight="1" spans="1:8">
       <c r="A10" s="10" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H10" s="11"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
       <c r="A11" s="13"/>
       <c r="B11" s="11" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H11" s="11"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:8">
       <c r="A12" s="14"/>
       <c r="B12" s="11" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H12" s="11"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
       <c r="A13" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -3689,7 +3721,7 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
       <selection pane="topRight" activeCell="C9" sqref="C9"/>
@@ -3702,7 +3734,7 @@
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3">
         <v>20220501</v>
@@ -3716,7 +3748,7 @@
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B2" s="6">
         <v>20220531</v>
@@ -3730,7 +3762,7 @@
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>1</v>
@@ -3748,15 +3780,15 @@
         <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
       <c r="A4" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
@@ -3766,7 +3798,7 @@
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H4" s="11"/>
     </row>
@@ -3774,13 +3806,13 @@
       <c r="A5" s="12"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H5" s="11"/>
     </row>
@@ -3788,7 +3820,7 @@
       <c r="A6" s="12"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -3800,7 +3832,7 @@
     </row>
     <row r="7" ht="13.65" customHeight="1" spans="1:8">
       <c r="A7" s="10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
@@ -3816,7 +3848,7 @@
       <c r="A8" s="13"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -3828,7 +3860,7 @@
       <c r="A9" s="14"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -3838,7 +3870,7 @@
     </row>
     <row r="10" ht="13.65" customHeight="1" spans="1:8">
       <c r="A10" s="10" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3870,7 +3902,7 @@
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
       <c r="A13" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>

</xml_diff>

<commit_message>
Site updated: 2024-06-14 15:12:25
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2023.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2023.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17020" activeTab="1"/>
+    <workbookView windowHeight="16440" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
@@ -12,13 +12,19 @@
     <sheet name="一月" sheetId="10" r:id="rId3"/>
     <sheet name="二月" sheetId="11" r:id="rId4"/>
     <sheet name="五月" sheetId="12" r:id="rId5"/>
+    <sheet name="十月" sheetId="13" r:id="rId6"/>
+    <sheet name="十一月" sheetId="14" r:id="rId7"/>
+    <sheet name="十二月" sheetId="15" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">待办任务!$A$1:$D$27</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="111">
   <si>
     <t>角色</t>
   </si>
@@ -77,12 +83,30 @@
     <t>同事</t>
   </si>
   <si>
+    <t>紧急程度状态</t>
+  </si>
+  <si>
+    <t>不重要不紧急</t>
+  </si>
+  <si>
+    <t>不重要紧急</t>
+  </si>
+  <si>
+    <t>重要不紧急</t>
+  </si>
+  <si>
+    <t>重要紧急</t>
+  </si>
+  <si>
     <t>任务名称</t>
   </si>
   <si>
     <t>说明</t>
   </si>
   <si>
+    <t>优先级</t>
+  </si>
+  <si>
     <t>状态</t>
   </si>
   <si>
@@ -122,10 +146,10 @@
     <t>通货膨胀一直在发生，如何抵御呢？</t>
   </si>
   <si>
-    <t>上海儿童福利</t>
-  </si>
-  <si>
-    <t>拥有居住证后，儿童可以在上海享受哪些福利？儿童医保/儿童互助基金…</t>
+    <t>上海儿童教育</t>
+  </si>
+  <si>
+    <t>在上海针对儿童教育需要提前做好哪些准备?</t>
   </si>
   <si>
     <t>思考是否要考公务员</t>
@@ -141,6 +165,116 @@
   </si>
   <si>
     <t>比如做投资人/up主，最好是自己感兴趣的。感兴趣的不一定能做好，但是不感兴趣的一定做不好</t>
+  </si>
+  <si>
+    <t>本质问题是普通人如何抓住ai的风口?如何适应ai改造后的社会?如何利用好ai改变自己和生活?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color indexed="8"/>
+        <rFont val="pingfang sc"/>
+        <charset val="134"/>
+      </rPr>
+      <t>推动时代发展的技术</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color indexed="8"/>
+        <rFont val="pingfang sc"/>
+        <charset val="134"/>
+      </rPr>
+      <t>领域</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color indexed="8"/>
+        <rFont val="pingfang sc"/>
+        <charset val="134"/>
+      </rPr>
+      <t>行业</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color indexed="8"/>
+        <rFont val="pingfang sc"/>
+        <charset val="134"/>
+      </rPr>
+      <t>方向是什么</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+        <charset val="134"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color indexed="8"/>
+        <rFont val="pingfang sc"/>
+        <charset val="134"/>
+      </rPr>
+      <t>普通人如何紧跟</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+        <charset val="134"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>上海考编</t>
+  </si>
+  <si>
+    <t>详细调研+开始学习+参加24年事业单位考试</t>
+  </si>
+  <si>
+    <t>央企/国企/私企</t>
+  </si>
+  <si>
+    <t>确定目标+面试技巧调研（一岗位一简历）+面试学习准备</t>
+  </si>
+  <si>
+    <t>进行中</t>
   </si>
   <si>
     <t>面部保养</t>
@@ -173,9 +307,6 @@
     <t>研究透彻设计模式（50%）、jvm考点系统性梳理、多线程实战场景梳理</t>
   </si>
   <si>
-    <t>进行中</t>
-  </si>
-  <si>
     <t>研究透彻业务设计模式DDD、研究透彻设计模式（50%）</t>
   </si>
   <si>
@@ -188,16 +319,22 @@
     <t>学习知识点“精”、“简”</t>
   </si>
   <si>
-    <t>mac电脑学习备忘整理</t>
+    <t>学习备忘整理</t>
+  </si>
+  <si>
+    <t>mac电脑中记录的学习备忘需要整理推进</t>
   </si>
   <si>
     <t>如何拥有健康的身体</t>
   </si>
   <si>
+    <t>作息、饮食等</t>
+  </si>
+  <si>
     <t>如何了解自己</t>
   </si>
   <si>
-    <t>如何利用ai改变行业</t>
+    <t>回答为什么要了解自己?如何了解自己?自己是个怎样的人?自己想要什么?</t>
   </si>
   <si>
     <t>开始时间:</t>
@@ -282,6 +419,36 @@
   </si>
   <si>
     <t>看5篇知识点</t>
+  </si>
+  <si>
+    <t>确定央企目标</t>
+  </si>
+  <si>
+    <t>调研如何进入央企</t>
+  </si>
+  <si>
+    <t>调研央企面试技术点</t>
+  </si>
+  <si>
+    <t>完成龙系统团队功能改造</t>
+  </si>
+  <si>
+    <t>jvm学习</t>
+  </si>
+  <si>
+    <t>jvm体系梳理完成</t>
+  </si>
+  <si>
+    <t>有那些好用且强大的ai工具</t>
+  </si>
+  <si>
+    <t>调研完成上海考编报考/学习资料</t>
+  </si>
+  <si>
+    <t>jvm现有视屏整理完成</t>
+  </si>
+  <si>
+    <t>年终总结</t>
   </si>
 </sst>
 </file>
@@ -289,12 +456,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -324,11 +491,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9.75"/>
+      <color indexed="8"/>
+      <name val="pingfang sc"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <color rgb="FFFF0000"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -338,10 +510,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -352,19 +541,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -386,7 +566,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -400,9 +596,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -415,14 +610,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
@@ -430,9 +617,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -446,23 +640,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -474,8 +653,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.75"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="41">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -496,12 +681,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="25"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -514,7 +693,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="25"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="16"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.15"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,7 +717,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,7 +747,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,13 +771,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,7 +783,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,25 +801,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,61 +849,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,25 +879,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -712,7 +915,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,6 +932,36 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -795,21 +1034,6 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="13"/>
       </left>
       <right/>
@@ -856,21 +1080,6 @@
         <color indexed="17"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="18"/>
-      </top>
       <bottom style="thin">
         <color indexed="13"/>
       </bottom>
@@ -1031,17 +1240,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1057,6 +1257,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1091,6 +1300,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1108,20 +1328,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1130,152 +1339,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1283,6 +1492,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1291,62 +1518,53 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1366,10 +1584,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1381,59 +1605,77 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2635,216 +2877,241 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.4230769230769" style="1" customWidth="1"/>
     <col min="2" max="16384" width="6" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:5">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:5">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:5">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
     </row>
     <row r="5" ht="14" customHeight="1" spans="1:5">
-      <c r="A5" s="52"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
     </row>
     <row r="6" ht="14" customHeight="1" spans="1:5">
-      <c r="A6" s="52"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:5">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
     </row>
     <row r="8" ht="14" customHeight="1" spans="1:5">
-      <c r="A8" s="52"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:5">
-      <c r="A9" s="52"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
     </row>
     <row r="10" ht="14" customHeight="1" spans="1:5">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
     </row>
     <row r="11" ht="14" customHeight="1" spans="1:5">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:5">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
     </row>
     <row r="13" ht="14" customHeight="1" spans="1:5">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:5">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:5">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:5">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
     </row>
     <row r="17" ht="14" customHeight="1" spans="1:5">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
     </row>
     <row r="18" ht="14" customHeight="1" spans="1:5">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
     </row>
     <row r="19" ht="14" customHeight="1" spans="1:5">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
     </row>
     <row r="20" ht="14" customHeight="1" spans="1:5">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
     </row>
     <row r="21" ht="14" customHeight="1" spans="1:5">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
     </row>
     <row r="22" ht="14" customHeight="1" spans="1:5">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
     </row>
     <row r="23" ht="14" customHeight="1" spans="1:5">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+    </row>
+    <row r="26" customHeight="1" spans="1:1">
+      <c r="A26" s="63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:1">
+      <c r="A27" s="35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" customHeight="1" spans="1:1">
+      <c r="A28" s="50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" customHeight="1" spans="1:1">
+      <c r="A29" s="40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" customHeight="1" spans="1:1">
+      <c r="A30" s="33" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2864,255 +3131,386 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="16.3557692307692" style="1" customWidth="1"/>
-    <col min="2" max="2" width="99.1153846153846" style="24" customWidth="1"/>
-    <col min="3" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
+    <col min="2" max="2" width="99.1153846153846" style="27" customWidth="1"/>
+    <col min="3" max="3" width="14.1057692307692" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A1" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="26" t="s">
+    <row r="1" ht="13.55" customHeight="1" spans="1:4">
+      <c r="A1" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" ht="13.35" customHeight="1" spans="1:4">
+      <c r="A2" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" ht="13.35" customHeight="1" spans="1:4">
+      <c r="A3" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D3" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" ht="13.35" customHeight="1" spans="1:4">
+      <c r="A4" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" ht="13.35" customHeight="1" spans="1:4">
+      <c r="A5" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" ht="13.35" customHeight="1" spans="1:4">
+      <c r="A6" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" ht="13.35" customHeight="1" spans="1:4">
+      <c r="A7" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" ht="13.35" customHeight="1" spans="1:4">
+      <c r="A8" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" ht="13.35" customHeight="1" spans="1:4">
+      <c r="A9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" ht="13.35" customHeight="1" spans="1:4">
+      <c r="A10" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:4">
+      <c r="A11" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:4">
+      <c r="A12" s="44"/>
+      <c r="B12" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:4">
+      <c r="A13" s="44"/>
+      <c r="B13" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:4">
+      <c r="A14" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:4">
+      <c r="A15" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:4">
+      <c r="A16" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="50" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A2" s="28" t="s">
+      <c r="D16" s="46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:4">
+      <c r="A17" s="49"/>
+      <c r="B17" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:4">
+      <c r="A18" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="D18" s="53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" ht="73" customHeight="1" spans="1:4">
+      <c r="A19" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A3" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A4" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A5" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A6" s="34" t="s">
+      <c r="D19" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A7" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="29" t="s">
+    </row>
+    <row r="20" customHeight="1" spans="1:4">
+      <c r="A20" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="1:4">
+      <c r="A21" s="44"/>
+      <c r="B21" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A8" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A9" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A10" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" customHeight="1" spans="1:3">
-      <c r="A11" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" customHeight="1" spans="1:3">
-      <c r="A12" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:3">
-      <c r="A13" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" customHeight="1" spans="1:3">
-      <c r="A14" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" ht="73" customHeight="1" spans="1:3">
-      <c r="A15" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="45" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" customHeight="1" spans="1:3">
-      <c r="A16" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" customHeight="1" spans="1:3">
-      <c r="A17" s="46"/>
-      <c r="B17" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" customHeight="1" spans="1:3">
-      <c r="A18" s="46"/>
-      <c r="B18" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" customHeight="1" spans="1:3">
-      <c r="A19" s="46"/>
-      <c r="B19" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" customHeight="1" spans="1:3">
-      <c r="A20" s="46"/>
-      <c r="B20" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" customHeight="1" spans="2:2">
-      <c r="B21" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" customHeight="1" spans="2:2">
-      <c r="B22" s="24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" customHeight="1" spans="2:2">
-      <c r="B23" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" customHeight="1" spans="2:2">
-      <c r="B24" s="24" t="s">
-        <v>58</v>
+    </row>
+    <row r="22" customHeight="1" spans="1:4">
+      <c r="A22" s="44"/>
+      <c r="B22" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" customHeight="1" spans="1:4">
+      <c r="A23" s="44"/>
+      <c r="B23" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="56"/>
+      <c r="D23" s="57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" customHeight="1" spans="1:4">
+      <c r="A24" s="44"/>
+      <c r="B24" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" customHeight="1" spans="1:4">
+      <c r="A25" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:4">
+      <c r="A26" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:4">
+      <c r="A27" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A16:A20"/>
+  <autoFilter ref="A1:D27">
+    <extLst/>
+  </autoFilter>
+  <mergeCells count="4">
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="C20:C24"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C7 C8 C9 C15 C16 C17 C18 C19 C20 C2:C5 C10:C14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D19 D20 D21 D22 D23 D24 D25 D26 D27 D2:D5 D16:D18">
       <formula1>"未进行,进行中,已暂停,已完成"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3143,300 +3541,300 @@
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
-      <c r="A1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="3">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="9">
         <v>20220401</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
-      <c r="A2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="A2" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="25">
         <v>20220430</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
-      <c r="A3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>63</v>
+      <c r="G3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A4" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="11"/>
+      <c r="A4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A5" s="12"/>
-      <c r="B5" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="11"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A6" s="12"/>
-      <c r="B6" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="11"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A7" s="12"/>
-      <c r="B7" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="11"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A8" s="23"/>
-      <c r="B8" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="11"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" s="11"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A10" s="12"/>
-      <c r="B10" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="11"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A11" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="11"/>
+      <c r="A11" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A12" s="13"/>
-      <c r="B12" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="11"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A13" s="14"/>
-      <c r="B13" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="11"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A14" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="11"/>
+      <c r="A14" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A15" s="13"/>
-      <c r="B15" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="11"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:8">
-      <c r="A16" s="14"/>
-      <c r="B16" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="11"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A17" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="11"/>
+      <c r="A17" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A18" s="13"/>
-      <c r="B18" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="11"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A19" s="14"/>
-      <c r="B19" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="11"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A20" s="15"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3472,232 +3870,232 @@
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
-      <c r="A1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="3">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="9">
         <v>20220401</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
-      <c r="A2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="A2" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="25">
         <v>20220430</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
-      <c r="A3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>63</v>
+      <c r="G3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A4" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="11"/>
+      <c r="A4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A5" s="12"/>
-      <c r="B5" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="11"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A6" s="12"/>
-      <c r="B6" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="11"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A7" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="11"/>
+      <c r="A7" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A8" s="13"/>
-      <c r="B8" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="11"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A9" s="14"/>
-      <c r="B9" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="11"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A10" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" s="11"/>
+      <c r="A10" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A11" s="13"/>
-      <c r="B11" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="11"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:8">
-      <c r="A12" s="14"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A13" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="A13" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A14" s="13"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A15" s="14"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A16" s="15"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3724,7 +4122,7 @@
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="C9" sqref="C9"/>
+      <selection pane="topRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
@@ -3733,214 +4131,220 @@
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
-      <c r="A1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="3">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="9">
         <v>20220501</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
-      <c r="A2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="A2" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="25">
         <v>20220531</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
-      <c r="A3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>63</v>
+      <c r="G3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A4" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="11"/>
+      <c r="A4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A5" s="12"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="11"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A6" s="12"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="11"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A7" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="A7" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A8" s="13"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A9" s="14"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A10" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="A10" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A11" s="13"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:8">
-      <c r="A12" s="14"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A13" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="A13" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A14" s="13"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A15" s="14"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A16" s="15"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3960,4 +4364,736 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="2" width="16.3557692307692" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.8173076923077" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14" customHeight="1" spans="1:8">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="9">
+        <v>20231001</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" ht="14" customHeight="1" spans="1:8">
+      <c r="A2" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="9">
+        <v>20231031</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" ht="14" customHeight="1" spans="1:8">
+      <c r="A3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A5" s="16"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A6" s="16"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A7" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A8" s="17"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A9" s="18"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A10" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A11" s="17"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" ht="14" customHeight="1" spans="1:8">
+      <c r="A12" s="18"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" ht="14" customHeight="1" spans="1:8">
+      <c r="A13" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A14" s="15"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A15" s="16"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A16" s="19"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A17" s="20"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13 G14 G15">
+      <formula1>"未进行,进行中,已暂停,已完成"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="2" width="16.3557692307692" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.8173076923077" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14" customHeight="1" spans="1:8">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="9">
+        <v>20231001</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" ht="14" customHeight="1" spans="1:8">
+      <c r="A2" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="9">
+        <v>20231031</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" ht="14" customHeight="1" spans="1:8">
+      <c r="A3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A5" s="16"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A6" s="16"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A7" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A8" s="17"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A9" s="18"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A10" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A11" s="17"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" ht="14" customHeight="1" spans="1:8">
+      <c r="A12" s="18"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" ht="14" customHeight="1" spans="1:8">
+      <c r="A13" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A14" s="15"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A15" s="16"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A16" s="19"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A17" s="20"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G5 G7 G13">
+      <formula1>"未进行,进行中,已暂停,已完成"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="2" width="16.3557692307692" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.8173076923077" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14" customHeight="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" ht="14" customHeight="1" spans="1:8">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" ht="14" customHeight="1" spans="1:8">
+      <c r="A11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" ht="13.65" customHeight="1" spans="1:8">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A14"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G12 G13">
+      <formula1>"未进行,进行中,已暂停,已完成"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>